<commit_message>
jagged array and 2d Array
</commit_message>
<xml_diff>
--- a/07 Arrays/Jagged.xlsx
+++ b/07 Arrays/Jagged.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\Rough\java\07 Arrays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9870F60-FC66-4FA8-B18A-49DFA476203E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D3FE2E-F49C-4BAD-8F5C-DD30E7DEA4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76C44925-9652-456A-837D-619F0E45C73D}"/>
   </bookViews>
@@ -25,18 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -101,13 +120,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0246BBD4-AA48-49B2-9D9D-B74E5632736D}">
-  <dimension ref="B2:H9"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="228" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="228" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,51 +464,89 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C9:E9"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>